<commit_message>
feat: adcionando arquivos e alterando pastas
</commit_message>
<xml_diff>
--- a/BackLog Produto/BACKLOG PRODUTO.xlsx
+++ b/BackLog Produto/BACKLOG PRODUTO.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erione Technologies\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erione Technologies\Pim-Terceiro-Semestre-1\BackLog Produto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75323F0A-FD93-4127-A707-377F86F32B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB94C3EF-AC16-4F10-906A-38E08E98434A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{382B0824-085F-46F6-8F9B-52819645303C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{382B0824-085F-46F6-8F9B-52819645303C}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="1" r:id="rId1"/>
     <sheet name="DAILY" sheetId="2" r:id="rId2"/>
+    <sheet name="Retrospectiva" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="147">
   <si>
     <t>PLANEJAMENTO</t>
   </si>
@@ -674,6 +675,27 @@
   <si>
     <t>FINALIZADO- TRABALAHAR NA PoC - CRUD ; Houve dificuldade na integração com o banco de dados.</t>
   </si>
+  <si>
+    <t>RETROSPECTIVA DA SPRINT</t>
+  </si>
+  <si>
+    <t>25-03-24 | Segunda-Feira</t>
+  </si>
+  <si>
+    <t>DATA:</t>
+  </si>
+  <si>
+    <t>08-04-24 | Segunda-Feira</t>
+  </si>
+  <si>
+    <t>Assunto:</t>
+  </si>
+  <si>
+    <t>Na retrospectiva foi acordado a reformulação dos Backlogs: Produto, Sprint e PIM. E também reformulado o repositório do GitHub (organização etc).</t>
+  </si>
+  <si>
+    <t>Na retrospectiva for acordado a reformulação do backlog da entrega da Sprint, mudar nome do backlog-sprint. Colocar o que cada pessoa vai fazer no Trello, separar cada componente do grupo e criar pasta dentro da /backlog e colocar um arquivo com o grupo separado.</t>
+  </si>
 </sst>
 </file>
 
@@ -755,7 +777,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,8 +838,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1264,11 +1292,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1391,88 +1441,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1495,6 +1472,96 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1831,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21C7278-4439-4CF1-82AD-0D14D81CCEDD}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1850,31 +1917,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="80"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:10" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="77"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="41" t="s">
@@ -1886,7 +1953,7 @@
       <c r="B8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="76" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="22"/>
@@ -1904,15 +1971,15 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="215" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="82"/>
-      <c r="B9" s="98" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="74" t="s">
         <v>56</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="75" t="s">
         <v>93</v>
       </c>
       <c r="F9" s="51" t="s">
@@ -1926,7 +1993,7 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="215" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="82"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="14" t="s">
         <v>57</v>
       </c>
@@ -1948,7 +2015,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="82"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="14" t="s">
         <v>58</v>
       </c>
@@ -1991,7 +2058,7 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="14" t="s">
         <v>60</v>
       </c>
@@ -2013,7 +2080,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="146" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="82"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="14" t="s">
         <v>62</v>
       </c>
@@ -2035,7 +2102,7 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="179.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="14" t="s">
         <v>63</v>
       </c>
@@ -2078,7 +2145,7 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="225.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="82"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="14" t="s">
         <v>65</v>
       </c>
@@ -2161,7 +2228,7 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="82"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="14" t="s">
         <v>69</v>
       </c>
@@ -2225,7 +2292,7 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="82"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="14" t="s">
         <v>112</v>
       </c>
@@ -2285,12 +2352,12 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="G31" s="69" t="s">
+      <c r="G31" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="71"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="94"/>
     </row>
     <row r="32" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="6"/>
@@ -2315,10 +2382,10 @@
         <v>103</v>
       </c>
       <c r="H33" s="31"/>
-      <c r="I33" s="63" t="s">
+      <c r="I33" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="J33" s="64"/>
+      <c r="J33" s="87"/>
     </row>
     <row r="34" spans="2:10" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="6"/>
@@ -2329,8 +2396,8 @@
         <v>104</v>
       </c>
       <c r="H34" s="31"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="66"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="89"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C35" s="6"/>
@@ -2341,8 +2408,8 @@
         <v>81</v>
       </c>
       <c r="H35" s="31"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="66"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="89"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C36" s="6"/>
@@ -2353,8 +2420,8 @@
         <v>82</v>
       </c>
       <c r="H36" s="31"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="89"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
@@ -2365,8 +2432,8 @@
         <v>83</v>
       </c>
       <c r="H37" s="31"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="66"/>
+      <c r="I37" s="88"/>
+      <c r="J37" s="89"/>
     </row>
     <row r="38" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="6"/>
@@ -2377,8 +2444,8 @@
         <v>84</v>
       </c>
       <c r="H38" s="31"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="68"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="91"/>
     </row>
     <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="6"/>
@@ -2416,16 +2483,16 @@
       <c r="G43" s="6"/>
     </row>
     <row r="44" spans="2:10" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="74"/>
+      <c r="C44" s="96"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="97"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C45" s="6"/>
@@ -2450,16 +2517,16 @@
     </row>
     <row r="48" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="49" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B49" s="60" t="s">
+      <c r="B49" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="62"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="84"/>
+      <c r="I49" s="85"/>
     </row>
     <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="35"/>
@@ -2601,16 +2668,16 @@
     </row>
     <row r="58" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="59" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="61"/>
-      <c r="I59" s="62"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="85"/>
     </row>
     <row r="60" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B60" s="35"/>
@@ -2728,16 +2795,16 @@
     </row>
     <row r="67" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="68" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B68" s="60" t="s">
+      <c r="B68" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-      <c r="G68" s="61"/>
-      <c r="H68" s="61"/>
-      <c r="I68" s="62"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="84"/>
+      <c r="I68" s="85"/>
     </row>
     <row r="69" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B69" s="35"/>
@@ -2833,16 +2900,16 @@
     </row>
     <row r="75" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="76" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B76" s="60" t="s">
+      <c r="B76" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="61"/>
-      <c r="H76" s="61"/>
-      <c r="I76" s="62"/>
+      <c r="C76" s="84"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="84"/>
+      <c r="F76" s="84"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="84"/>
+      <c r="I76" s="85"/>
     </row>
     <row r="77" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B77" s="35"/>
@@ -2964,25 +3031,19 @@
     </row>
     <row r="84" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="85" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B85" s="60" t="s">
+      <c r="B85" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="C85" s="61"/>
-      <c r="D85" s="61"/>
-      <c r="E85" s="61"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="61"/>
-      <c r="H85" s="61"/>
-      <c r="I85" s="62"/>
+      <c r="C85" s="84"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="84"/>
+      <c r="F85" s="84"/>
+      <c r="G85" s="84"/>
+      <c r="H85" s="84"/>
+      <c r="I85" s="85"/>
     </row>
     <row r="86" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B86" s="35"/>
-      <c r="C86" s="81"/>
-      <c r="D86" s="81"/>
-      <c r="E86" s="81"/>
-      <c r="F86" s="81"/>
-      <c r="G86" s="81"/>
-      <c r="H86" s="81"/>
       <c r="I86" s="24"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.35">
@@ -3107,306 +3168,306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="85"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="61" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="86">
+      <c r="A3" s="63">
         <v>45405</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="64" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="86">
+      <c r="A4" s="63">
         <v>45405</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="64" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="86">
+      <c r="A5" s="63">
         <v>45405</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="64" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="86">
+      <c r="A6" s="63">
         <v>45405</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="C6" s="64" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="86">
+      <c r="A7" s="63">
         <v>45405</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="64" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="86">
+      <c r="A8" s="63">
         <v>45405</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="64" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="88"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="89"/>
+      <c r="A9" s="98"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="100"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="86">
+      <c r="A10" s="63">
         <v>45406</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="64" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="86">
+      <c r="A11" s="63">
         <v>45406</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="64" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="86">
+      <c r="A12" s="63">
         <v>45406</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="64" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="86">
+      <c r="A13" s="63">
         <v>45406</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="64" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="86">
+      <c r="A14" s="63">
         <v>45406</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="64" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="86">
+      <c r="A15" s="63">
         <v>45406</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="64" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="90"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="93">
+      <c r="A17" s="68">
         <v>45407</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="64" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="93">
+      <c r="A18" s="68">
         <v>45407</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="64" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="93">
+      <c r="A19" s="68">
         <v>45407</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="87" t="s">
+      <c r="C19" s="64" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="93">
+      <c r="A20" s="68">
         <v>45407</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="64" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="93">
+      <c r="A21" s="68">
         <v>45407</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="64" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="93">
+      <c r="A22" s="68">
         <v>45407</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="64" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="94"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="92"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="67"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="93">
+      <c r="A24" s="68">
         <v>45408</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="64" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="93">
+      <c r="A25" s="68">
         <v>45408</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="64" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="93">
+      <c r="A26" s="68">
         <v>45408</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="64" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="93">
+      <c r="A27" s="68">
         <v>45408</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="64" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="93">
+      <c r="A28" s="68">
         <v>45408</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="64" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="95">
+      <c r="A29" s="70">
         <v>45408</v>
       </c>
-      <c r="B29" s="96" t="s">
+      <c r="B29" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="97" t="s">
+      <c r="C29" s="72" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="92"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="54">
@@ -3415,7 +3476,7 @@
       <c r="B31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="64" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3426,7 +3487,7 @@
       <c r="B32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="87" t="s">
+      <c r="C32" s="64" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3437,7 +3498,7 @@
       <c r="B33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="64" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3448,7 +3509,7 @@
       <c r="B34" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="64" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3459,7 +3520,7 @@
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="87" t="s">
+      <c r="C35" s="64" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3467,17 +3528,17 @@
       <c r="A36" s="54">
         <v>45409</v>
       </c>
-      <c r="B36" s="96" t="s">
+      <c r="B36" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="97" t="s">
+      <c r="C36" s="72" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="92"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="67"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="54">
@@ -3486,7 +3547,7 @@
       <c r="B38" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="87" t="s">
+      <c r="C38" s="64" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3497,7 +3558,7 @@
       <c r="B39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="87" t="s">
+      <c r="C39" s="64" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3508,7 +3569,7 @@
       <c r="B40" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="64" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3519,7 +3580,7 @@
       <c r="B41" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="87" t="s">
+      <c r="C41" s="64" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3530,7 +3591,7 @@
       <c r="B42" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="87" t="s">
+      <c r="C42" s="64" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3538,17 +3599,17 @@
       <c r="A43" s="54">
         <v>45410</v>
       </c>
-      <c r="B43" s="96" t="s">
+      <c r="B43" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="97" t="s">
+      <c r="C43" s="72" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="92"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3557,4 +3618,66 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F06579-E269-4EF9-B570-7E87B660141A}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="55.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="102" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="105" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="106" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>